<commit_message>
Add Bootstrap e index
</commit_message>
<xml_diff>
--- a/arquivos_temp/Alunos.xlsx
+++ b/arquivos_temp/Alunos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DTI-GRC\Documents\Bruno\Dev\Univesp_PI_2024_1\arquivos_temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39504384-AFB5-45E0-BF42-327B87491668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE00D39-9E18-4BCC-9275-F31103EAB86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9F7689B1-1AFD-4EF7-9FBB-57502D5E640C}"/>
   </bookViews>
@@ -587,7 +587,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>